<commit_message>
Categories default now checked
</commit_message>
<xml_diff>
--- a/NerdQuiz_TODO.xlsx
+++ b/NerdQuiz_TODO.xlsx
@@ -23,7 +23,7 @@
     <t>Datenbank</t>
   </si>
   <si>
-    <t>Übernommen von </t>
+    <t>Übernommen von</t>
   </si>
   <si>
     <t>Status</t>
@@ -64,30 +64,33 @@
     <t>Lia</t>
   </si>
   <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Optional: Letzte Settings für Checked/Unchecked auslesen</t>
+  </si>
+  <si>
+    <t>StartGame Button implementieren</t>
+  </si>
+  <si>
+    <t>c)</t>
+  </si>
+  <si>
+    <t>Datenbankanbindung für die Kategorien implementieren</t>
+  </si>
+  <si>
+    <t>HighscoresActivity</t>
+  </si>
+  <si>
+    <t>Allgemeine Impelementierung</t>
+  </si>
+  <si>
+    <t>Alex</t>
+  </si>
+  <si>
     <t>In Progress</t>
   </si>
   <si>
-    <t>Optional: Letzte Settings für Checked/Unchecked auslesen</t>
-  </si>
-  <si>
-    <t>StartGame Button implementieren</t>
-  </si>
-  <si>
-    <t>c)</t>
-  </si>
-  <si>
-    <t>Datenbankanbindung für die Kategorien implementieren</t>
-  </si>
-  <si>
-    <t>HighscoresActivity</t>
-  </si>
-  <si>
-    <t>Allgemeine Impelementierung</t>
-  </si>
-  <si>
-    <t>Alex</t>
-  </si>
-  <si>
     <t>Datenbankanbindung</t>
   </si>
   <si>
@@ -100,9 +103,6 @@
     <t>Axel</t>
   </si>
   <si>
-    <t>Done</t>
-  </si>
-  <si>
     <t>Verknüpfung mit der Highscore Liste</t>
   </si>
   <si>
@@ -121,7 +121,7 @@
     <t>e)</t>
   </si>
   <si>
-    <t>Methode zum prüfen ob alle Fragen gespielt wurden </t>
+    <t>Methode zum prüfen ob alle Fragen gespielt wurden</t>
   </si>
   <si>
     <t>f)</t>
@@ -348,7 +348,7 @@
     <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
     <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
     <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
-    <cellStyle builtinId="54" customBuiltin="true" name="Excel Built-in Input" xfId="20"/>
+    <cellStyle builtinId="54" customBuiltin="true" name="Excel Built-in Excel Built-in Input" xfId="20"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -421,7 +421,7 @@
   <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
-      <selection activeCell="C10" activeCellId="0" pane="topLeft" sqref="C10"/>
+      <selection activeCell="D9" activeCellId="0" pane="topLeft" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -563,7 +563,7 @@
         <v>19</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="17">
@@ -571,7 +571,7 @@
         <v>6</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="18">
@@ -586,7 +586,7 @@
         <v>0</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>2</v>
@@ -600,13 +600,13 @@
         <v>4</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="22">
@@ -620,7 +620,7 @@
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="23">
       <c r="A23" s="7"/>
       <c r="B23" s="6" t="e">
-        <f aca="false">&gt; dialog fehlt der zugriff auf 'StartGameActivity' - eigener intent zur highscoreactivity?</f>
+        <f aca="false">&gt; dialog fehlt der zugriff auf 'startgameactivity' - eigener intent zur highscoreactivity?</f>
         <v>#VALUE!</v>
       </c>
     </row>

</xml_diff>